<commit_message>
'Time' -> 'time' in csv files; I'm not at all sure what I changed in the tag definitions file, but the current version looks right, so...
</commit_message>
<xml_diff>
--- a/docs/src/tags-documentation/Tag definitions.xlsx
+++ b/docs/src/tags-documentation/Tag definitions.xlsx
@@ -650,8 +650,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
-      <selection activeCell="A45" sqref="A45"/>
+    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1008,7 +1008,7 @@
         <v>53</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C33" s="2" t="s">
         <v>71</v>

</xml_diff>